<commit_message>
[200~Atualiza o arquivo excell com as soluções do AG
</commit_message>
<xml_diff>
--- a/algoritmo_genetico/Melhores de cada geração.xlsx
+++ b/algoritmo_genetico/Melhores de cada geração.xlsx
@@ -478,23 +478,23 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>3.644029232529793</v>
+        <v>10.09099863626659</v>
       </c>
       <c r="D2" t="n">
-        <v>6.426117182021622</v>
+        <v>6.110205640751736</v>
       </c>
       <c r="E2" t="n">
-        <v>95.30716790537663</v>
+        <v>91.86568587054964</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9926069767441861</v>
+        <v>2.683024242424243</v>
       </c>
       <c r="G2" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>{'Fe2O3': 9, 'CaO': 3, 'B2O3': 10, 'Nb2O5': 4, 'Mn2O3': 7, 'Li2SO4': 10, 'BaSO4': 6, 'CO2': 8, 'LiNO3': 9, 'CdSO4': 10, 'KNO3': 1, 'C6H12O6': 5, 'CaCO3': 4}</t>
+          <t>{'Bi2O3': 1, 'Cu2O': 1, 'CeO2': 6, 'MnO2': 10, 'CrO3': 6, '(NH4)2SO4': 2, 'SeO2': 3, 'HgO': 1, 'BaSO4': 1, 'CO2': 2}</t>
         </is>
       </c>
     </row>
@@ -506,23 +506,23 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9627014946693876</v>
+        <v>3.150893567858989</v>
       </c>
       <c r="D3" t="n">
-        <v>8.867958309753316</v>
+        <v>7.259688659482732</v>
       </c>
       <c r="E3" t="n">
-        <v>113.7955397801543</v>
+        <v>67.88668387469194</v>
       </c>
       <c r="F3" t="n">
-        <v>0.3003529411764706</v>
+        <v>0.8855833333333334</v>
       </c>
       <c r="G3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>{'Li2CO3': 6, 'Ca(NO3)2': 6, 'AlPO4': 5}</t>
+          <t>{'As2O3': 4, 'Co2O3': 6, 'Ca(NO3)2': 7, 'KNO3': 7}</t>
         </is>
       </c>
     </row>

</xml_diff>